<commit_message>
Oval and Line finished
</commit_message>
<xml_diff>
--- a/funciton command list.xlsx
+++ b/funciton command list.xlsx
@@ -331,43 +331,43 @@
     <t xml:space="preserve">CallIf SectionName </t>
   </si>
   <si>
+    <t xml:space="preserve">0.26190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnterCritical </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SetDrawFlash 0x100 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CallIfNot SectionName </t>
+  </si>
+  <si>
     <t xml:space="preserve">WaitInput 111 SimPickle SimTriggerSecondDetent </t>
   </si>
   <si>
-    <t xml:space="preserve">0.26190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EnterCritical </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SetDrawFlash 0x100 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallIfNot SectionName </t>
+    <t xml:space="preserve">0.27063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EndCritical </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SetFont 1 </t>
   </si>
   <si>
     <t xml:space="preserve">Hilite3DButton 10 SimICPAG </t>
   </si>
   <si>
-    <t xml:space="preserve">0.27063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndCritical </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SetFont 1 </t>
+    <t xml:space="preserve">0.27936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SetFontBGColor 0xFFFFFFFF </t>
   </si>
   <si>
     <t xml:space="preserve">WaitHilite3DButton 10 SimICPAG </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.27936</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SetFontBGColor 0xFFFFFFFF </t>
   </si>
   <si>
     <t xml:space="preserve">0.28809</t>
@@ -5385,7 +5385,7 @@
   <dimension ref="A2:XFD193"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6125,61 +6125,62 @@
       <c r="E33" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>103</v>
-      </c>
+      <c r="F33" s="0"/>
       <c r="L33" s="6" t="n">
         <v>150</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="E34" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="F34" s="21" t="s">
         <v>107</v>
-      </c>
-      <c r="F34" s="21" t="s">
-        <v>108</v>
       </c>
       <c r="L34" s="6" t="n">
         <v>155</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="F35" s="21" t="s">
         <v>111</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>112</v>
       </c>
       <c r="L35" s="6" t="n">
         <v>160</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="F36" s="21" t="s">
         <v>115</v>
       </c>
       <c r="L36" s="6" t="n">

</xml_diff>